<commit_message>
ver 3.3 リリース (#53)
</commit_message>
<xml_diff>
--- a/サンプルプロジェクト/設計書/A1_プロジェクト管理システム/030_アプリ設計/010_システム機能設計/システム処理フロー_A1_プロジェクト管理システム.xlsx
+++ b/サンプルプロジェクト/設計書/A1_プロジェクト管理システム/030_アプリ設計/010_システム機能設計/システム処理フロー_A1_プロジェクト管理システム.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57302F9-18EA-4326-BE4C-97F8B9AEE1B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA11A3EE-3730-48A7-A669-C68DD3AF8330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="75" windowWidth="38400" windowHeight="10575" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="20" r:id="rId1"/>
@@ -28,15 +28,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">変更履歴!$1:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">目次!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -6434,10 +6426,10 @@
       <xdr:rowOff>60107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>100013</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>138114</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6449,18 +6441,18 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="96" idx="0"/>
+          <a:stCxn id="93" idx="3"/>
           <a:endCxn id="9" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
+        <a:xfrm flipH="1" flipV="1">
           <a:off x="4848219" y="2803307"/>
-          <a:ext cx="1328744" cy="1363882"/>
+          <a:ext cx="1971681" cy="1078131"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -122759"/>
+            <a:gd name="adj1" fmla="val -11594"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -6490,16 +6482,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6516,7 +6508,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7248525" y="3924300"/>
+          <a:off x="7162800" y="3724275"/>
           <a:ext cx="542925" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9914,7 +9906,7 @@
                 <a:latin typeface="ＭＳ 明朝"/>
                 <a:ea typeface="ＭＳ 明朝"/>
               </a:rPr>
-              <a:t>プロジェクト照会</a:t>
+              <a:t>プロジェクト検索</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -10605,7 +10597,7 @@
                 <a:latin typeface="ＭＳ 明朝"/>
                 <a:ea typeface="ＭＳ 明朝"/>
               </a:rPr>
-              <a:t>WA10203WA</a:t>
+              <a:t>WA10203</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -14948,7 +14940,7 @@
               <a:latin typeface="ＭＳ 明朝"/>
               <a:ea typeface="ＭＳ 明朝"/>
             </a:rPr>
-            <a:t>期間内プロジェクト一覧出力バッチ</a:t>
+            <a:t>プロジェクト一覧出力</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>

</xml_diff>